<commit_message>
moved mobile-check to displayservice, isMobile is subscribable behavioussubject
</commit_message>
<xml_diff>
--- a/Schablonen/PathologyVergleich.xlsx
+++ b/Schablonen/PathologyVergleich.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maste\Git\radiospeech\Schablonen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ECA7E741-8FA4-4A29-BBF0-FA504C0CD540}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B57EED0D-31DD-4310-B13B-5ACA0A54484C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Zwei-Ebenen-Thorax" sheetId="2" r:id="rId1"/>
-    <sheet name="Intensivlungen - Andreas" sheetId="3" r:id="rId2"/>
-    <sheet name="Intensivlungen - Hamo" sheetId="1" r:id="rId3"/>
+    <sheet name="Zwei-Ebenen-Thorax - Ver. 1" sheetId="2" r:id="rId1"/>
+    <sheet name="Zwei-Ebenen-Thorax - Ver. 2" sheetId="4" r:id="rId2"/>
+    <sheet name="Intensivlungen - Ver. 1" sheetId="3" r:id="rId3"/>
+    <sheet name="Intensivlungen - Ver. 2" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="67">
   <si>
     <t>Gliederung</t>
   </si>
@@ -220,6 +221,9 @@
   </si>
   <si>
     <t>Hiatushernie</t>
+  </si>
+  <si>
+    <t>Rundherd</t>
   </si>
 </sst>
 </file>
@@ -1541,7 +1545,7 @@
   <dimension ref="A1:O103"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3491,11 +3495,348 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE938BA5-D1E6-446C-BC47-3B5FBB1CF019}">
-  <dimension ref="A1:O110"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68862737-AAB2-4104-969A-AD52C03DDD38}">
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="34.85546875" customWidth="1"/>
+    <col min="4" max="4" width="69.7109375" customWidth="1"/>
+    <col min="5" max="5" width="4.140625" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" customWidth="1"/>
+    <col min="7" max="7" width="4.5703125" customWidth="1"/>
+    <col min="8" max="8" width="3" customWidth="1"/>
+    <col min="9" max="9" width="3.85546875" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" customWidth="1"/>
+    <col min="11" max="12" width="56.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="4.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J8" t="s">
+        <v>50</v>
+      </c>
+      <c r="K8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="C10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="C11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="C15" t="s">
+        <v>36</v>
+      </c>
+      <c r="D15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="17" spans="3:12">
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" t="s">
+        <v>38</v>
+      </c>
+      <c r="J17" t="s">
+        <v>39</v>
+      </c>
+      <c r="K17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="3:12">
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="19" spans="3:12">
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" t="s">
+        <v>59</v>
+      </c>
+      <c r="J19" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" t="s">
+        <v>48</v>
+      </c>
+      <c r="L19" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="3:12">
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="3:12">
+      <c r="C21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="3:12">
+      <c r="C22" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="3:12">
+      <c r="C23" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="24" spans="3:12">
+      <c r="C24" t="s">
+        <v>52</v>
+      </c>
+      <c r="D24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="3:12">
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="3:12">
+      <c r="C26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE938BA5-D1E6-446C-BC47-3B5FBB1CF019}">
+  <dimension ref="A1:O99"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -3918,7 +4259,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
     </row>
-    <row r="17" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="17" spans="1:15" ht="14.45" customHeight="1">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2" t="s">
@@ -3939,7 +4280,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
     </row>
-    <row r="18" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="18" spans="1:15" ht="14.45" customHeight="1">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
       <c r="C18" s="2" t="s">
@@ -3966,7 +4307,7 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
     </row>
-    <row r="19" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="19" spans="1:15" ht="14.45" customHeight="1">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
@@ -3983,7 +4324,7 @@
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
     </row>
-    <row r="20" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="20" spans="1:15" ht="14.45" customHeight="1">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="2"/>
@@ -4000,7 +4341,7 @@
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
     </row>
-    <row r="21" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="21" spans="1:15" ht="14.45" customHeight="1">
       <c r="A21" s="3"/>
       <c r="B21" s="3"/>
       <c r="C21" s="2"/>
@@ -4017,7 +4358,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="3"/>
     </row>
-    <row r="22" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="22" spans="1:15" ht="14.45" customHeight="1">
       <c r="A22" s="3"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -4034,7 +4375,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
     </row>
-    <row r="23" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="23" spans="1:15" ht="14.45" customHeight="1">
       <c r="A23" s="3"/>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -4051,7 +4392,7 @@
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
     </row>
-    <row r="24" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="24" spans="1:15" ht="14.45" customHeight="1">
       <c r="A24" s="3"/>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -4068,7 +4409,7 @@
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
     </row>
-    <row r="25" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="25" spans="1:15" ht="14.45" customHeight="1">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -4085,7 +4426,7 @@
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
-    <row r="26" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="26" spans="1:15" ht="14.45" customHeight="1">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -4102,7 +4443,7 @@
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
-    <row r="27" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="27" spans="1:15" ht="14.45" customHeight="1">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -4119,7 +4460,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
     </row>
-    <row r="28" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="28" spans="1:15" ht="14.45" customHeight="1">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -4136,7 +4477,7 @@
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
     </row>
-    <row r="29" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="29" spans="1:15" ht="14.45" customHeight="1">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -4153,7 +4494,7 @@
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
     </row>
-    <row r="30" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="30" spans="1:15" ht="14.45" customHeight="1">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -4170,7 +4511,7 @@
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
     </row>
-    <row r="31" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="31" spans="1:15" ht="14.45" customHeight="1">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -4187,7 +4528,7 @@
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
     </row>
-    <row r="32" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="32" spans="1:15" ht="14.45" customHeight="1">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -4204,7 +4545,7 @@
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
     </row>
-    <row r="33" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="33" spans="1:15" ht="14.45" customHeight="1">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -4221,7 +4562,7 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
     </row>
-    <row r="34" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="34" spans="1:15" ht="14.45" customHeight="1">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -4238,7 +4579,7 @@
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
     </row>
-    <row r="35" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="35" spans="1:15" ht="14.45" customHeight="1">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -4255,7 +4596,7 @@
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
     </row>
-    <row r="36" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="36" spans="1:15" ht="14.45" customHeight="1">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -4272,7 +4613,7 @@
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
     </row>
-    <row r="37" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="37" spans="1:15" ht="14.45" customHeight="1">
       <c r="A37" s="3"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -4289,7 +4630,7 @@
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
     </row>
-    <row r="38" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="38" spans="1:15" ht="14.45" customHeight="1">
       <c r="A38" s="3"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -4306,7 +4647,7 @@
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
     </row>
-    <row r="39" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="39" spans="1:15" ht="14.45" customHeight="1">
       <c r="A39" s="3"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -4323,7 +4664,7 @@
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
     </row>
-    <row r="40" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="40" spans="1:15" ht="14.45" customHeight="1">
       <c r="A40" s="3"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
@@ -4340,7 +4681,7 @@
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
     </row>
-    <row r="41" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="41" spans="1:15" ht="14.45" customHeight="1">
       <c r="A41" s="3"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -4357,7 +4698,7 @@
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
     </row>
-    <row r="42" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="42" spans="1:15" ht="14.45" customHeight="1">
       <c r="A42" s="3"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -4374,7 +4715,7 @@
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
     </row>
-    <row r="43" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="43" spans="1:15" ht="14.45" customHeight="1">
       <c r="A43" s="3"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
@@ -4391,7 +4732,7 @@
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
     </row>
-    <row r="44" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="44" spans="1:15" ht="14.45" customHeight="1">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -4408,7 +4749,7 @@
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
     </row>
-    <row r="45" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="45" spans="1:15" ht="14.45" customHeight="1">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -4425,7 +4766,7 @@
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
     </row>
-    <row r="46" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="46" spans="1:15" ht="14.45" customHeight="1">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -4442,7 +4783,7 @@
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
     </row>
-    <row r="47" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="47" spans="1:15" ht="14.45" customHeight="1">
       <c r="A47" s="3"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
@@ -4459,7 +4800,7 @@
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
     </row>
-    <row r="48" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="48" spans="1:15" ht="14.45" customHeight="1">
       <c r="A48" s="3"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -4476,7 +4817,7 @@
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
     </row>
-    <row r="49" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="49" spans="1:15" ht="14.45" customHeight="1">
       <c r="A49" s="3"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -4493,7 +4834,7 @@
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
     </row>
-    <row r="50" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="50" spans="1:15" ht="14.45" customHeight="1">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -4510,7 +4851,7 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
     </row>
-    <row r="51" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="51" spans="1:15" ht="14.45" customHeight="1">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4527,7 +4868,7 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
     </row>
-    <row r="52" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="52" spans="1:15" ht="14.45" customHeight="1">
       <c r="A52" s="3"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
@@ -4544,7 +4885,7 @@
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
     </row>
-    <row r="53" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="53" spans="1:15" ht="14.45" customHeight="1">
       <c r="A53" s="3"/>
       <c r="B53" s="3"/>
       <c r="C53" s="3"/>
@@ -4561,7 +4902,7 @@
       <c r="N53" s="3"/>
       <c r="O53" s="3"/>
     </row>
-    <row r="54" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="54" spans="1:15" ht="14.45" customHeight="1">
       <c r="A54" s="3"/>
       <c r="B54" s="3"/>
       <c r="C54" s="3"/>
@@ -4578,7 +4919,7 @@
       <c r="N54" s="3"/>
       <c r="O54" s="3"/>
     </row>
-    <row r="55" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="55" spans="1:15" ht="14.45" customHeight="1">
       <c r="A55" s="3"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3"/>
@@ -4595,7 +4936,7 @@
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
     </row>
-    <row r="56" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="56" spans="1:15" ht="14.45" customHeight="1">
       <c r="A56" s="3"/>
       <c r="B56" s="3"/>
       <c r="C56" s="3"/>
@@ -4612,7 +4953,7 @@
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
     </row>
-    <row r="57" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="57" spans="1:15" ht="14.45" customHeight="1">
       <c r="A57" s="3"/>
       <c r="B57" s="3"/>
       <c r="C57" s="3"/>
@@ -4629,7 +4970,7 @@
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
     </row>
-    <row r="58" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="58" spans="1:15" ht="14.45" customHeight="1">
       <c r="A58" s="3"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
@@ -4646,7 +4987,7 @@
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
     </row>
-    <row r="59" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="59" spans="1:15" ht="14.45" customHeight="1">
       <c r="A59" s="3"/>
       <c r="B59" s="3"/>
       <c r="C59" s="3"/>
@@ -4663,7 +5004,7 @@
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
     </row>
-    <row r="60" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="60" spans="1:15" ht="14.45" customHeight="1">
       <c r="A60" s="3"/>
       <c r="B60" s="3"/>
       <c r="C60" s="3"/>
@@ -4680,7 +5021,7 @@
       <c r="N60" s="5"/>
       <c r="O60" s="3"/>
     </row>
-    <row r="61" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="61" spans="1:15" ht="14.45" customHeight="1">
       <c r="A61" s="3"/>
       <c r="B61" s="3"/>
       <c r="C61" s="3"/>
@@ -4697,7 +5038,7 @@
       <c r="N61" s="7"/>
       <c r="O61" s="8"/>
     </row>
-    <row r="62" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="62" spans="1:15" ht="14.45" customHeight="1">
       <c r="A62" s="3"/>
       <c r="B62" s="3"/>
       <c r="C62" s="3"/>
@@ -4714,7 +5055,7 @@
       <c r="N62" s="9"/>
       <c r="O62" s="3"/>
     </row>
-    <row r="63" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="63" spans="1:15" ht="14.45" customHeight="1">
       <c r="A63" s="3"/>
       <c r="B63" s="3"/>
       <c r="C63" s="3"/>
@@ -4731,7 +5072,7 @@
       <c r="N63" s="7"/>
       <c r="O63" s="8"/>
     </row>
-    <row r="64" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="64" spans="1:15" ht="14.45" customHeight="1">
       <c r="A64" s="3"/>
       <c r="B64" s="3"/>
       <c r="C64" s="3"/>
@@ -4748,7 +5089,7 @@
       <c r="N64" s="7"/>
       <c r="O64" s="8"/>
     </row>
-    <row r="65" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="65" spans="1:15" ht="14.45" customHeight="1">
       <c r="A65" s="3"/>
       <c r="B65" s="3"/>
       <c r="C65" s="3"/>
@@ -4765,7 +5106,7 @@
       <c r="N65" s="7"/>
       <c r="O65" s="8"/>
     </row>
-    <row r="66" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="66" spans="1:15" ht="14.45" customHeight="1">
       <c r="A66" s="3"/>
       <c r="B66" s="3"/>
       <c r="C66" s="3"/>
@@ -4782,7 +5123,7 @@
       <c r="N66" s="7"/>
       <c r="O66" s="8"/>
     </row>
-    <row r="67" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="67" spans="1:15" ht="14.45" customHeight="1">
       <c r="A67" s="3"/>
       <c r="B67" s="3"/>
       <c r="C67" s="3"/>
@@ -4799,7 +5140,7 @@
       <c r="N67" s="7"/>
       <c r="O67" s="8"/>
     </row>
-    <row r="68" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="68" spans="1:15" ht="14.45" customHeight="1">
       <c r="A68" s="3"/>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
@@ -4816,7 +5157,7 @@
       <c r="N68" s="11"/>
       <c r="O68" s="3"/>
     </row>
-    <row r="69" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="69" spans="1:15" ht="14.45" customHeight="1">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
@@ -4833,7 +5174,7 @@
       <c r="N69" s="3"/>
       <c r="O69" s="3"/>
     </row>
-    <row r="70" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="70" spans="1:15" ht="14.45" customHeight="1">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
       <c r="C70" s="3"/>
@@ -4850,7 +5191,7 @@
       <c r="N70" s="3"/>
       <c r="O70" s="3"/>
     </row>
-    <row r="71" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="71" spans="1:15" ht="14.45" customHeight="1">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
       <c r="C71" s="3"/>
@@ -4867,7 +5208,7 @@
       <c r="N71" s="3"/>
       <c r="O71" s="3"/>
     </row>
-    <row r="72" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="72" spans="1:15" ht="14.45" customHeight="1">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
       <c r="C72" s="3"/>
@@ -4884,7 +5225,7 @@
       <c r="N72" s="3"/>
       <c r="O72" s="3"/>
     </row>
-    <row r="73" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="73" spans="1:15" ht="14.45" customHeight="1">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
       <c r="C73" s="3"/>
@@ -4901,7 +5242,7 @@
       <c r="N73" s="3"/>
       <c r="O73" s="3"/>
     </row>
-    <row r="74" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="74" spans="1:15" ht="14.45" customHeight="1">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
       <c r="C74" s="3"/>
@@ -4918,7 +5259,7 @@
       <c r="N74" s="3"/>
       <c r="O74" s="3"/>
     </row>
-    <row r="75" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="75" spans="1:15" ht="14.45" customHeight="1">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -4935,7 +5276,7 @@
       <c r="N75" s="3"/>
       <c r="O75" s="3"/>
     </row>
-    <row r="76" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="76" spans="1:15" ht="14.45" customHeight="1">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -4952,7 +5293,7 @@
       <c r="N76" s="3"/>
       <c r="O76" s="3"/>
     </row>
-    <row r="77" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="77" spans="1:15" ht="14.45" customHeight="1">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -4969,7 +5310,7 @@
       <c r="N77" s="3"/>
       <c r="O77" s="3"/>
     </row>
-    <row r="78" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="78" spans="1:15" ht="14.45" customHeight="1">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -4986,7 +5327,7 @@
       <c r="N78" s="3"/>
       <c r="O78" s="3"/>
     </row>
-    <row r="79" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="79" spans="1:15" ht="14.45" customHeight="1">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5003,7 +5344,7 @@
       <c r="N79" s="3"/>
       <c r="O79" s="3"/>
     </row>
-    <row r="80" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="80" spans="1:15" ht="14.45" customHeight="1">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -5020,7 +5361,7 @@
       <c r="N80" s="3"/>
       <c r="O80" s="3"/>
     </row>
-    <row r="81" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="81" spans="1:15" ht="14.45" customHeight="1">
       <c r="A81" s="3"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -5037,7 +5378,7 @@
       <c r="N81" s="3"/>
       <c r="O81" s="3"/>
     </row>
-    <row r="82" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="82" spans="1:15" ht="14.45" customHeight="1">
       <c r="A82" s="3"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -5054,7 +5395,7 @@
       <c r="N82" s="3"/>
       <c r="O82" s="3"/>
     </row>
-    <row r="83" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="83" spans="1:15" ht="14.45" customHeight="1">
       <c r="A83" s="3"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -5071,7 +5412,7 @@
       <c r="N83" s="3"/>
       <c r="O83" s="3"/>
     </row>
-    <row r="84" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="84" spans="1:15" ht="14.45" customHeight="1">
       <c r="A84" s="3"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -5088,7 +5429,7 @@
       <c r="N84" s="3"/>
       <c r="O84" s="3"/>
     </row>
-    <row r="85" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="85" spans="1:15" ht="14.45" customHeight="1">
       <c r="A85" s="3"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -5105,7 +5446,7 @@
       <c r="N85" s="3"/>
       <c r="O85" s="3"/>
     </row>
-    <row r="86" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="86" spans="1:15" ht="14.45" customHeight="1">
       <c r="A86" s="3"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -5122,7 +5463,7 @@
       <c r="N86" s="3"/>
       <c r="O86" s="3"/>
     </row>
-    <row r="87" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="87" spans="1:15" ht="14.45" customHeight="1">
       <c r="A87" s="3"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -5139,7 +5480,7 @@
       <c r="N87" s="3"/>
       <c r="O87" s="3"/>
     </row>
-    <row r="88" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="88" spans="1:15" ht="14.45" customHeight="1">
       <c r="A88" s="3"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -5156,7 +5497,7 @@
       <c r="N88" s="3"/>
       <c r="O88" s="3"/>
     </row>
-    <row r="89" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="89" spans="1:15" ht="14.45" customHeight="1">
       <c r="A89" s="3"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -5173,7 +5514,7 @@
       <c r="N89" s="3"/>
       <c r="O89" s="3"/>
     </row>
-    <row r="90" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="90" spans="1:15" ht="14.45" customHeight="1">
       <c r="A90" s="3"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -5190,7 +5531,7 @@
       <c r="N90" s="3"/>
       <c r="O90" s="3"/>
     </row>
-    <row r="91" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="91" spans="1:15" ht="14.45" customHeight="1">
       <c r="A91" s="3"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -5207,7 +5548,7 @@
       <c r="N91" s="3"/>
       <c r="O91" s="3"/>
     </row>
-    <row r="92" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="92" spans="1:15" ht="14.45" customHeight="1">
       <c r="A92" s="3"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -5224,7 +5565,7 @@
       <c r="N92" s="3"/>
       <c r="O92" s="3"/>
     </row>
-    <row r="93" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="93" spans="1:15" ht="14.45" customHeight="1">
       <c r="A93" s="3"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -5241,7 +5582,7 @@
       <c r="N93" s="3"/>
       <c r="O93" s="3"/>
     </row>
-    <row r="94" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="94" spans="1:15" ht="14.45" customHeight="1">
       <c r="A94" s="3"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -5258,7 +5599,7 @@
       <c r="N94" s="3"/>
       <c r="O94" s="3"/>
     </row>
-    <row r="95" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="95" spans="1:15" ht="14.45" customHeight="1">
       <c r="A95" s="3"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -5275,7 +5616,7 @@
       <c r="N95" s="3"/>
       <c r="O95" s="3"/>
     </row>
-    <row r="96" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="96" spans="1:15" ht="14.45" customHeight="1">
       <c r="A96" s="3"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -5292,7 +5633,7 @@
       <c r="N96" s="3"/>
       <c r="O96" s="3"/>
     </row>
-    <row r="97" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="97" spans="1:15" ht="14.45" customHeight="1">
       <c r="A97" s="3"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -5309,7 +5650,7 @@
       <c r="N97" s="3"/>
       <c r="O97" s="3"/>
     </row>
-    <row r="98" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="98" spans="1:15" ht="14.45" customHeight="1">
       <c r="A98" s="3"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -5326,7 +5667,7 @@
       <c r="N98" s="3"/>
       <c r="O98" s="3"/>
     </row>
-    <row r="99" spans="1:15" s="1" customFormat="1" ht="14.45" customHeight="1">
+    <row r="99" spans="1:15" ht="14.45" customHeight="1">
       <c r="A99" s="3"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -5343,28 +5684,17 @@
       <c r="N99" s="3"/>
       <c r="O99" s="3"/>
     </row>
-    <row r="100" spans="1:15" s="1" customFormat="1"/>
-    <row r="101" spans="1:15" s="1" customFormat="1"/>
-    <row r="102" spans="1:15" s="1" customFormat="1"/>
-    <row r="103" spans="1:15" s="1" customFormat="1"/>
-    <row r="104" spans="1:15" s="1" customFormat="1"/>
-    <row r="105" spans="1:15" s="1" customFormat="1"/>
-    <row r="106" spans="1:15" s="1" customFormat="1"/>
-    <row r="107" spans="1:15" s="1" customFormat="1"/>
-    <row r="108" spans="1:15" s="1" customFormat="1"/>
-    <row r="109" spans="1:15" s="1" customFormat="1"/>
-    <row r="110" spans="1:15" s="1" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O88"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="14.45" customHeight="1"/>
@@ -5373,16 +5703,16 @@
     <col min="2" max="2" width="8.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="26.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="115.7109375" style="1" customWidth="1"/>
-    <col min="5" max="6" width="7" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="13.42578125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="40.42578125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="68.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="26.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="170.85546875" style="1" customWidth="1"/>
-    <col min="15" max="15" width="81.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="7" style="1" customWidth="1"/>
+    <col min="6" max="6" width="2.140625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="3.28515625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="3" style="1" customWidth="1"/>
+    <col min="10" max="10" width="3.5703125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="3.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="2.7109375" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6" style="1" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.7109375" style="1" customWidth="1"/>
     <col min="16" max="16" width="8.85546875" style="1" customWidth="1"/>
     <col min="17" max="16384" width="8.85546875" style="1"/>
   </cols>

</xml_diff>